<commit_message>
ajustes rotulos de dados e proporcao
</commit_message>
<xml_diff>
--- a/base_vendas.xlsx
+++ b/base_vendas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\Bootcamp Santander\_Projetos\Criando Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1BD4B4-B575-4519-896E-C7468E0CA37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01693491-4DC9-47C7-82D6-56F61736B120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28665" yWindow="-135" windowWidth="29070" windowHeight="16020" firstSheet="3" activeTab="3" xr2:uid="{28DD5B76-0634-4F87-BE60-8BFA7EF2E23B}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2061" uniqueCount="333">
   <si>
     <t>Paleta de Cores</t>
   </si>
@@ -1142,6 +1142,9 @@
   </si>
   <si>
     <t>XBOX GAMES PASS SUBSCRIPTION SALES</t>
+  </si>
+  <si>
+    <t>(Vários itens)</t>
   </si>
   <si>
     <t xml:space="preserve">EA Play Season Pass </t>
@@ -1308,7 +1311,13 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16"/>
   </cellStyles>
-  <dxfs count="118">
+  <dxfs count="120">
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="34" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     </dxf>
@@ -1681,8 +1690,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Segmentação de Dados 1" pivot="0" table="0" count="4" xr9:uid="{939C61F8-B2DA-47C9-9FE9-1C65515A4C3B}">
-      <tableStyleElement type="wholeTable" dxfId="99"/>
-      <tableStyleElement type="headerRow" dxfId="98"/>
+      <tableStyleElement type="wholeTable" dxfId="101"/>
+      <tableStyleElement type="headerRow" dxfId="100"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1968,8 +1977,9 @@
               <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2010,6 +2020,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>C̳álculos!$C$8:$C$11</c:f>
@@ -2034,13 +2102,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>101</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>96</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2388,7 +2456,9 @@
         <c:idx val="2"/>
         <c:spPr>
           <a:solidFill>
-            <a:srgbClr val="5BF6A8"/>
+            <a:srgbClr val="5BF6A8">
+              <a:alpha val="98000"/>
+            </a:srgbClr>
           </a:solidFill>
           <a:ln>
             <a:noFill/>
@@ -2429,8 +2499,9 @@
               <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2463,7 +2534,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="5BF6A8"/>
+              <a:srgbClr val="5BF6A8">
+                <a:alpha val="98000"/>
+              </a:srgbClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2471,6 +2544,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>C̳álculos!$C$19:$C$21</c:f>
@@ -2492,10 +2623,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>147</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>148</c:v>
+                  <c:v>102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2507,8 +2638,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="inBase"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2527,7 +2659,7 @@
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -2574,16 +2706,19 @@
         <c:axId val="2035392240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="160"/>
+          <c:min val="100"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="359943040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="10"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2883,8 +3018,9 @@
               <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2925,6 +3061,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>C̳álculos!$C$29:$C$31</c:f>
@@ -2946,10 +3140,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>197</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3337,8 +3531,9 @@
               <a:endParaRPr lang="pt-BR"/>
             </a:p>
           </c:txPr>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -3379,6 +3574,64 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="pt-BR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>C̳álculos!$G$8:$G$10</c:f>
@@ -3400,10 +3653,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>101</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>194</c:v>
+                  <c:v>134</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4194,13 +4447,13 @@
                 <c:formatCode>_("R$"* #,##0.00_);_("R$"* \(#,##0.00\);_("R$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>505</c:v>
+                  <c:v>345</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>960</c:v>
+                  <c:v>660</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1470</c:v>
+                  <c:v>1020</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4265,7 +4518,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2940</c:v>
+                  <c:v>2040</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4327,10 +4580,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1920</c:v>
+                  <c:v>1320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1960</c:v>
+                  <c:v>1360</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8339,7 +8592,7 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>472440</xdr:colOff>
@@ -8377,7 +8630,7 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
@@ -8415,7 +8668,7 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>459105</xdr:colOff>
@@ -8453,7 +8706,7 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>478155</xdr:colOff>
@@ -13927,9 +14180,9 @@
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
@@ -13998,7 +14251,7 @@
     <dataField name="Minecraft Season Pass " fld="12" baseField="2" baseItem="0" numFmtId="44"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="101">
+    <format dxfId="103">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -14008,7 +14261,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="100">
+    <format dxfId="102">
       <pivotArea field="2" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisRow" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -14018,34 +14271,7 @@
       </pivotArea>
     </format>
   </formats>
-  <chartFormats count="6">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
+  <chartFormats count="3">
     <chartFormat chart="4" format="6" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -14112,9 +14338,9 @@
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
@@ -14184,16 +14410,7 @@
   <dataFields count="1">
     <dataField name="Contagem de Minecraft Season Pass" fld="11" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
+  <chartFormats count="1">
     <chartFormat chart="4" format="2" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -14217,7 +14434,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A05AA8A-A031-46F2-8061-A5699356F9F4}" name="tbl_ea_season_pass" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A05AA8A-A031-46F2-8061-A5699356F9F4}" name="tbl_ea_season_pass" cacheId="37" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="C28:D31" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="15">
     <pivotField showAll="0"/>
@@ -14242,9 +14459,9 @@
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
@@ -14363,9 +14580,9 @@
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
@@ -14472,9 +14689,9 @@
         <item x="1"/>
         <item x="2"/>
         <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
         <item x="7"/>
         <item x="8"/>
         <item x="9"/>
@@ -14885,9 +15102,9 @@
         <i x="1" s="1"/>
         <i x="2" s="1"/>
         <i x="3" s="1"/>
-        <i x="4" s="1"/>
-        <i x="5" s="1"/>
-        <i x="6" s="1"/>
+        <i x="4"/>
+        <i x="5"/>
+        <i x="6"/>
         <i x="7" s="1"/>
         <i x="8" s="1"/>
         <i x="9" s="1"/>
@@ -14929,7 +15146,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:O296" totalsRowShown="0" dataDxfId="117">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}" name="Tabela1" displayName="Tabela1" ref="A1:O296" totalsRowShown="0" dataDxfId="119">
   <autoFilter ref="A1:O296" xr:uid="{34E0E886-4200-4B36-97B3-63DB74FF40A0}">
     <filterColumn colId="11">
       <filters>
@@ -14938,25 +15155,25 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="116"/>
-    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="115"/>
-    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="114"/>
-    <tableColumn id="15" xr3:uid="{E07C5652-2E5C-49E6-BFC9-ACE3165B74D6}" name="Year" dataDxfId="102">
+    <tableColumn id="1" xr3:uid="{C4A90516-688A-46BF-9167-EA16C2A8A652}" name="Subscriber ID" dataDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{53DD39D0-2220-4121-9E9D-4EAA7E151C0F}" name="Name" dataDxfId="117"/>
+    <tableColumn id="3" xr3:uid="{4F5FF271-4C57-4BE0-8F2C-F82C8551625C}" name="Plan" dataDxfId="116"/>
+    <tableColumn id="15" xr3:uid="{E07C5652-2E5C-49E6-BFC9-ACE3165B74D6}" name="Year" dataDxfId="104">
       <calculatedColumnFormula>YEAR(Tabela1[[#This Row],[Start Date]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{815015B2-DAAA-4F70-9275-94435043B58C}" name="Month" dataDxfId="103">
+    <tableColumn id="14" xr3:uid="{815015B2-DAAA-4F70-9275-94435043B58C}" name="Month" dataDxfId="105">
       <calculatedColumnFormula>CONCATENATE(TEXT(MONTH(Tabela1[[#This Row],[Start Date]]),"00"),"/",YEAR(Tabela1[[#This Row],[Start Date]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="113"/>
-    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="112"/>
-    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="111" dataCellStyle="Moeda"/>
-    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="110"/>
-    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="109"/>
-    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="108" dataCellStyle="Moeda"/>
-    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="107"/>
-    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="106" dataCellStyle="Moeda"/>
-    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="105" dataCellStyle="Moeda"/>
-    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="104" dataCellStyle="Moeda"/>
+    <tableColumn id="4" xr3:uid="{8C17EB93-79B9-4E55-B8F7-BEB82F8253E9}" name="Start Date" dataDxfId="115"/>
+    <tableColumn id="5" xr3:uid="{48CEDF9B-1689-482A-A828-5CCE7713264A}" name="Auto Renewal" dataDxfId="114"/>
+    <tableColumn id="6" xr3:uid="{78B82374-9AA7-4E38-AE4F-78CDE6C83720}" name="Subscription Price" dataDxfId="113" dataCellStyle="Moeda"/>
+    <tableColumn id="7" xr3:uid="{F2433F68-AF33-49D0-B1FB-19A396074EDE}" name="Subscription Type" dataDxfId="112"/>
+    <tableColumn id="8" xr3:uid="{FD4D9C95-F6E5-4933-9068-A71FF7DF9343}" name="EA Play Season Pass" dataDxfId="111"/>
+    <tableColumn id="13" xr3:uid="{978DD0D2-834E-4CE4-A39B-30976086932F}" name="EA Play Season Pass_x000a_Price" dataDxfId="110" dataCellStyle="Moeda"/>
+    <tableColumn id="9" xr3:uid="{6E29F111-C395-4580-9DAD-3407D9E8B1A4}" name="Minecraft Season Pass" dataDxfId="109"/>
+    <tableColumn id="10" xr3:uid="{EF544EAA-7F25-4FD5-A10E-8E62804DB9E3}" name="Minecraft Season Pass Price" dataDxfId="108" dataCellStyle="Moeda"/>
+    <tableColumn id="11" xr3:uid="{7F6EB64A-1F07-4E48-9F0F-AC7D9DCD26F8}" name="Coupon Value" dataDxfId="107" dataCellStyle="Moeda"/>
+    <tableColumn id="12" xr3:uid="{2B04ABC8-DE6F-426E-ADC0-D8AFC68CA58E}" name="Total Value" dataDxfId="106" dataCellStyle="Moeda"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -30048,13 +30265,13 @@
         <v>317</v>
       </c>
       <c r="D4" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="G4" s="12" t="s">
         <v>317</v>
       </c>
       <c r="H4" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.3">
@@ -30090,13 +30307,13 @@
         <v>22</v>
       </c>
       <c r="D8" s="14">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="14">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.3">
@@ -30104,13 +30321,13 @@
         <v>26</v>
       </c>
       <c r="D9" s="14">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="14">
-        <v>194</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.3">
@@ -30118,13 +30335,13 @@
         <v>18</v>
       </c>
       <c r="D10" s="14">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>314</v>
       </c>
       <c r="H10" s="14">
-        <v>295</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.3">
@@ -30132,7 +30349,7 @@
         <v>314</v>
       </c>
       <c r="D11" s="14">
-        <v>295</v>
+        <v>203</v>
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.3">
@@ -30162,13 +30379,13 @@
         <v>317</v>
       </c>
       <c r="D15" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>317</v>
       </c>
       <c r="H15" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.3">
@@ -30196,13 +30413,13 @@
         <v>313</v>
       </c>
       <c r="H18" t="s">
+        <v>330</v>
+      </c>
+      <c r="I18" t="s">
         <v>329</v>
       </c>
-      <c r="I18" t="s">
-        <v>328</v>
-      </c>
       <c r="J18" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.3">
@@ -30210,13 +30427,13 @@
         <v>23</v>
       </c>
       <c r="D19" s="14">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="16">
-        <v>505</v>
+        <v>345</v>
       </c>
       <c r="I19" s="16">
         <v>0</v>
@@ -30230,19 +30447,19 @@
         <v>19</v>
       </c>
       <c r="D20" s="14">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>26</v>
       </c>
       <c r="H20" s="16">
-        <v>960</v>
+        <v>660</v>
       </c>
       <c r="I20" s="16">
         <v>0</v>
       </c>
       <c r="J20" s="16">
-        <v>1920</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.3">
@@ -30250,19 +30467,19 @@
         <v>314</v>
       </c>
       <c r="D21" s="14">
-        <v>295</v>
+        <v>203</v>
       </c>
       <c r="G21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="H21" s="16">
-        <v>1470</v>
+        <v>1020</v>
       </c>
       <c r="I21" s="16">
-        <v>2940</v>
+        <v>2040</v>
       </c>
       <c r="J21" s="16">
-        <v>1960</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.3">
@@ -30270,13 +30487,13 @@
         <v>314</v>
       </c>
       <c r="H22" s="16">
-        <v>2935</v>
+        <v>2025</v>
       </c>
       <c r="I22" s="16">
-        <v>2940</v>
+        <v>2040</v>
       </c>
       <c r="J22" s="16">
-        <v>3880</v>
+        <v>2680</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.3">
@@ -30297,7 +30514,7 @@
         <v>317</v>
       </c>
       <c r="D25" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.3">
@@ -30321,7 +30538,7 @@
         <v>23</v>
       </c>
       <c r="D29" s="14">
-        <v>197</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.3">
@@ -30329,7 +30546,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="14">
-        <v>98</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="3:10" x14ac:dyDescent="0.3">
@@ -30337,7 +30554,7 @@
         <v>314</v>
       </c>
       <c r="D31" s="14">
-        <v>295</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -30351,7 +30568,7 @@
   <dimension ref="A2:Z53"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30394,7 +30611,7 @@
     <row r="5" spans="1:26" s="7" customFormat="1" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="C5" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:26" s="7" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>